<commit_message>
added copy config in tmux
</commit_message>
<xml_diff>
--- a/emacs_cheatsheet.xlsx
+++ b/emacs_cheatsheet.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10830"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10928"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kanishk/Downloads/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kanishk/professional/configs/configs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{44A39303-77C6-4243-9798-41CDB3022B20}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{FD730E29-31E0-3941-9BB1-1685ABE1347E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4340" yWindow="500" windowWidth="24460" windowHeight="16940" xr2:uid="{DB0BB786-CC79-3246-8EE5-25725AD88A98}"/>
+    <workbookView xWindow="4420" yWindow="680" windowWidth="25820" windowHeight="18960" xr2:uid="{DB0BB786-CC79-3246-8EE5-25725AD88A98}"/>
   </bookViews>
   <sheets>
     <sheet name="emacs_cheatsheet" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="156" uniqueCount="117">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="170" uniqueCount="129">
   <si>
     <t>Command</t>
   </si>
@@ -371,13 +371,49 @@
   </si>
   <si>
     <t>publish branch</t>
+  </si>
+  <si>
+    <t>search and replace</t>
+  </si>
+  <si>
+    <t>C-x n n</t>
+  </si>
+  <si>
+    <t>Narrow to region</t>
+  </si>
+  <si>
+    <t>C-x n w</t>
+  </si>
+  <si>
+    <t>widen</t>
+  </si>
+  <si>
+    <t>functions</t>
+  </si>
+  <si>
+    <t>goto line</t>
+  </si>
+  <si>
+    <t>ag</t>
+  </si>
+  <si>
+    <t>undo-tree-visualisation</t>
+  </si>
+  <si>
+    <t>ace swap windows</t>
+  </si>
+  <si>
+    <t>C-x C-spc</t>
+  </si>
+  <si>
+    <t>go to previous mark</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="18" x14ac:knownFonts="1">
+  <fonts count="19" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -511,6 +547,12 @@
       <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="Aptos Narrow (Body)"/>
     </font>
   </fonts>
   <fills count="33">
@@ -854,8 +896,9 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1231,10 +1274,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FEC42473-9417-564E-94BB-C46BAE2BE950}">
-  <dimension ref="A1:C54"/>
+  <dimension ref="A1:C64"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="A57" sqref="A57"/>
+      <selection activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1359,21 +1402,21 @@
         <v>2</v>
       </c>
       <c r="B11" t="s">
-        <v>21</v>
+        <v>127</v>
       </c>
       <c r="C11" t="s">
-        <v>22</v>
+        <v>128</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>23</v>
+        <v>2</v>
       </c>
       <c r="B12" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="C12" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.2">
@@ -1381,10 +1424,10 @@
         <v>23</v>
       </c>
       <c r="B13" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="C13" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.2">
@@ -1392,10 +1435,10 @@
         <v>23</v>
       </c>
       <c r="B14" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="C14" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.2">
@@ -1403,21 +1446,21 @@
         <v>23</v>
       </c>
       <c r="B15" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="C15" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>32</v>
+        <v>23</v>
       </c>
       <c r="B16" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="C16" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.2">
@@ -1425,10 +1468,10 @@
         <v>32</v>
       </c>
       <c r="B17" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="C17" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.2">
@@ -1436,10 +1479,10 @@
         <v>32</v>
       </c>
       <c r="B18" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="C18" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.2">
@@ -1447,10 +1490,10 @@
         <v>32</v>
       </c>
       <c r="B19" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="C19" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.2">
@@ -1458,21 +1501,21 @@
         <v>32</v>
       </c>
       <c r="B20" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="C20" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>43</v>
+        <v>32</v>
       </c>
       <c r="B21" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="C21" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.2">
@@ -1480,10 +1523,10 @@
         <v>43</v>
       </c>
       <c r="B22" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="C22" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.2">
@@ -1491,10 +1534,10 @@
         <v>43</v>
       </c>
       <c r="B23" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="C23" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.2">
@@ -1502,21 +1545,21 @@
         <v>43</v>
       </c>
       <c r="B24" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="C24" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>52</v>
+        <v>43</v>
       </c>
       <c r="B25" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="C25" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.2">
@@ -1524,10 +1567,10 @@
         <v>52</v>
       </c>
       <c r="B26" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="C26" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.2">
@@ -1535,10 +1578,10 @@
         <v>52</v>
       </c>
       <c r="B27" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="C27" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.2">
@@ -1546,21 +1589,21 @@
         <v>52</v>
       </c>
       <c r="B28" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="C28" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>61</v>
+        <v>52</v>
       </c>
       <c r="B29" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="C29" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.2">
@@ -1568,10 +1611,10 @@
         <v>61</v>
       </c>
       <c r="B30" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="C30" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.2">
@@ -1579,21 +1622,21 @@
         <v>61</v>
       </c>
       <c r="B31" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="C31" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
-        <v>68</v>
+        <v>61</v>
       </c>
       <c r="B32" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="C32" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.2">
@@ -1601,10 +1644,10 @@
         <v>68</v>
       </c>
       <c r="B33" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="C33" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.2">
@@ -1612,10 +1655,10 @@
         <v>68</v>
       </c>
       <c r="B34" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="C34" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.2">
@@ -1623,43 +1666,43 @@
         <v>68</v>
       </c>
       <c r="B35" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="C35" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
-        <v>104</v>
+        <v>68</v>
       </c>
       <c r="B36" t="s">
-        <v>106</v>
+        <v>75</v>
       </c>
       <c r="C36" t="s">
-        <v>104</v>
+        <v>76</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
-        <v>78</v>
+        <v>104</v>
       </c>
       <c r="B37" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="C37" t="s">
-        <v>78</v>
+        <v>104</v>
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B38" t="s">
-        <v>80</v>
+        <v>105</v>
       </c>
       <c r="C38" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.2">
@@ -1667,10 +1710,10 @@
         <v>79</v>
       </c>
       <c r="B39" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="C39" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.2">
@@ -1678,43 +1721,43 @@
         <v>79</v>
       </c>
       <c r="B40" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="C40" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
+        <v>79</v>
+      </c>
+      <c r="B41" t="s">
+        <v>84</v>
+      </c>
+      <c r="C41" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A42" t="s">
         <v>89</v>
       </c>
-      <c r="B41" t="s">
+      <c r="B42" t="s">
         <v>90</v>
       </c>
-      <c r="C41" t="s">
+      <c r="C42" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A43" t="s">
+    <row r="44" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A44" t="s">
         <v>86</v>
       </c>
-      <c r="B43" t="s">
+      <c r="B44" t="s">
         <v>87</v>
       </c>
-      <c r="C43" t="s">
+      <c r="C44" t="s">
         <v>88</v>
-      </c>
-    </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A45" t="s">
-        <v>92</v>
-      </c>
-      <c r="B45" t="s">
-        <v>93</v>
-      </c>
-      <c r="C45" t="s">
-        <v>94</v>
       </c>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.2">
@@ -1722,10 +1765,10 @@
         <v>92</v>
       </c>
       <c r="B46" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="C46" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.2">
@@ -1733,32 +1776,32 @@
         <v>92</v>
       </c>
       <c r="B47" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="C47" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
-        <v>99</v>
+        <v>92</v>
       </c>
       <c r="B48" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="C48" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
-        <v>92</v>
+        <v>99</v>
       </c>
       <c r="B49" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="C49" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.2">
@@ -1766,54 +1809,112 @@
         <v>92</v>
       </c>
       <c r="B50" t="s">
-        <v>107</v>
+        <v>102</v>
       </c>
       <c r="C50" t="s">
-        <v>110</v>
+        <v>103</v>
       </c>
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
-        <v>99</v>
+        <v>92</v>
       </c>
       <c r="B51" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="C51" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
-        <v>92</v>
+        <v>99</v>
       </c>
       <c r="B52" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="C52" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
-        <v>99</v>
+        <v>92</v>
       </c>
       <c r="B53" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="C53" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
+        <v>99</v>
+      </c>
+      <c r="B54" t="s">
+        <v>113</v>
+      </c>
+      <c r="C54" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="55" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A55" t="s">
         <v>92</v>
       </c>
-      <c r="B54" t="s">
+      <c r="B55" t="s">
         <v>115</v>
       </c>
-      <c r="C54" t="s">
+      <c r="C55" t="s">
         <v>116</v>
+      </c>
+    </row>
+    <row r="57" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A57" t="s">
+        <v>117</v>
+      </c>
+      <c r="B57" t="s">
+        <v>118</v>
+      </c>
+      <c r="C57" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="58" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A58" t="s">
+        <v>117</v>
+      </c>
+      <c r="B58" t="s">
+        <v>120</v>
+      </c>
+      <c r="C58" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="60" spans="1:3" ht="19" x14ac:dyDescent="0.25">
+      <c r="A60" s="1" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="61" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A61" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="62" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A62" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="63" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A63" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="64" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A64" t="s">
+        <v>126</v>
       </c>
     </row>
   </sheetData>

</xml_diff>